<commit_message>
Drafted servo driver based on timer 2 with 2 channels. Test fails.
</commit_message>
<xml_diff>
--- a/doc/Cam Control Design.xlsx
+++ b/doc/Cam Control Design.xlsx
@@ -1,26 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\David\Documents\VSCode\stan-base\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C6C11E-55BE-4140-B1C3-85E3F3107ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Speed" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Clock Frequency (Hz)</t>
   </si>
@@ -53,19 +68,22 @@
   </si>
   <si>
     <t>PWM period error (%)</t>
+  </si>
+  <si>
+    <t>Tick duration (ns)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.000000"/>
-    <numFmt numFmtId="170" formatCode="0.0000000"/>
-    <numFmt numFmtId="172" formatCode="0.000000000"/>
-    <numFmt numFmtId="174" formatCode="0.0%"/>
-    <numFmt numFmtId="176" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000000"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -91,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,6 +119,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -118,26 +142,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
     <dxf>
-      <numFmt numFmtId="174" formatCode="0.0%"/>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.000000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -146,7 +191,16 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="0.0000%"/>
+      <numFmt numFmtId="167" formatCode="0.000000000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.0000%"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -155,7 +209,16 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="0.0000000"/>
+      <numFmt numFmtId="168" formatCode="0.0%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -164,14 +227,11 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="169" formatCode="0.000000"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -185,29 +245,11 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.000000000"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -242,34 +284,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:I11" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:I11"/>
-  <tableColumns count="9">
-    <tableColumn id="3" name="Prescaler idx" dataDxfId="8">
-      <calculatedColumnFormula>2*D2</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:J11" totalsRowShown="0" dataDxfId="10">
+  <autoFilter ref="A1:J11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Prescaler idx" dataDxfId="9">
+      <calculatedColumnFormula>2*E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Prescaler" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prescaler" dataDxfId="8">
       <calculatedColumnFormula>POWER(2,Tableau1[[#This Row],[Prescaler idx]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Tick duration (s)" dataDxfId="5">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tick duration (s)" dataDxfId="2">
       <calculatedColumnFormula>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="TOF Period (s)" dataDxfId="3">
+    <tableColumn id="10" xr3:uid="{C9857BCC-44A0-4A41-B3FE-4B20550591FB}" name="Tick duration (ns)" dataDxfId="0">
+      <calculatedColumnFormula>Tableau1[[#This Row],[Tick duration (s)]]*1000000000</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TOF Period (s)" dataDxfId="1">
       <calculatedColumnFormula>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1*256</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Number of TOF" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Number of TOF" dataDxfId="7">
       <calculatedColumnFormula>Constants!$B$2/Tableau1[[#This Row],[TOF Period (s)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Integer num TOF" dataDxfId="7">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Integer num TOF" dataDxfId="6">
       <calculatedColumnFormula>FLOOR(Tableau1[[#This Row],[Number of TOF]], 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Achievable period (s)" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Achievable period (s)" dataDxfId="5">
       <calculatedColumnFormula>Tableau1[[#This Row],[Integer num TOF]]*Tableau1[[#This Row],[TOF Period (s)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="PWM period error (%)" dataDxfId="0" dataCellStyle="Pourcentage">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PWM period error (%)" dataDxfId="4" dataCellStyle="Pourcentage">
       <calculatedColumnFormula>(Constants!$B$2-Tableau1[[#This Row],[Achievable period (s)]])/Constants!$B$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="PWM resolution (%)" dataDxfId="1" dataCellStyle="Pourcentage">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="PWM resolution (%)" dataDxfId="3" dataCellStyle="Pourcentage">
       <calculatedColumnFormula>Tableau1[[#This Row],[Tick duration (s)]]/Tableau1[[#This Row],[Achievable period (s)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -532,18 +577,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,15 +596,16 @@
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" customWidth="1"/>
-    <col min="9" max="9" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -570,25 +616,28 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -600,32 +649,36 @@
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1</f>
         <v>1.2499999999999999E-7</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="3">
+        <f>Tableau1[[#This Row],[Tick duration (s)]]*1000000000</f>
+        <v>125</v>
+      </c>
+      <c r="E2" s="8">
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1*256</f>
         <v>3.1999999999999999E-5</v>
       </c>
-      <c r="E2" s="5">
+      <c r="F2" s="5">
         <f>Constants!$B$2/Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>625</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <f>FLOOR(Tableau1[[#This Row],[Number of TOF]], 1)</f>
         <v>625</v>
       </c>
-      <c r="G2" s="6">
+      <c r="H2" s="6">
         <f>Tableau1[[#This Row],[Integer num TOF]]*Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>0.02</v>
       </c>
-      <c r="H2" s="9">
+      <c r="I2" s="9">
         <f>(Constants!$B$2-Tableau1[[#This Row],[Achievable period (s)]])/Constants!$B$2</f>
         <v>0</v>
       </c>
-      <c r="I2" s="10">
+      <c r="J2" s="10">
         <f>Tableau1[[#This Row],[Tick duration (s)]]/Tableau1[[#This Row],[Achievable period (s)]]</f>
         <v>6.2499999999999995E-6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -637,32 +690,36 @@
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1</f>
         <v>2.4999999999999999E-7</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="3">
+        <f>Tableau1[[#This Row],[Tick duration (s)]]*1000000000</f>
+        <v>250</v>
+      </c>
+      <c r="E3" s="8">
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1*256</f>
         <v>6.3999999999999997E-5</v>
       </c>
-      <c r="E3" s="5">
+      <c r="F3" s="5">
         <f>Constants!$B$2/Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>312.5</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <f>FLOOR(Tableau1[[#This Row],[Number of TOF]], 1)</f>
         <v>312</v>
       </c>
-      <c r="G3" s="6">
+      <c r="H3" s="6">
         <f>Tableau1[[#This Row],[Integer num TOF]]*Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>1.9968E-2</v>
       </c>
-      <c r="H3" s="9">
+      <c r="I3" s="9">
         <f>(Constants!$B$2-Tableau1[[#This Row],[Achievable period (s)]])/Constants!$B$2</f>
         <v>1.6000000000000389E-3</v>
       </c>
-      <c r="I3" s="10">
+      <c r="J3" s="10">
         <f>Tableau1[[#This Row],[Tick duration (s)]]/Tableau1[[#This Row],[Achievable period (s)]]</f>
         <v>1.2520032051282051E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -674,32 +731,36 @@
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1</f>
         <v>4.9999999999999998E-7</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="3">
+        <f>Tableau1[[#This Row],[Tick duration (s)]]*1000000000</f>
+        <v>500</v>
+      </c>
+      <c r="E4" s="8">
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1*256</f>
         <v>1.2799999999999999E-4</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
         <f>Constants!$B$2/Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>156.25</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <f>FLOOR(Tableau1[[#This Row],[Number of TOF]], 1)</f>
         <v>156</v>
       </c>
-      <c r="G4" s="6">
+      <c r="H4" s="6">
         <f>Tableau1[[#This Row],[Integer num TOF]]*Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>1.9968E-2</v>
       </c>
-      <c r="H4" s="9">
+      <c r="I4" s="9">
         <f>(Constants!$B$2-Tableau1[[#This Row],[Achievable period (s)]])/Constants!$B$2</f>
         <v>1.6000000000000389E-3</v>
       </c>
-      <c r="I4" s="10">
+      <c r="J4" s="10">
         <f>Tableau1[[#This Row],[Tick duration (s)]]/Tableau1[[#This Row],[Achievable period (s)]]</f>
         <v>2.5040064102564102E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -711,69 +772,77 @@
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="3">
+        <f>Tableau1[[#This Row],[Tick duration (s)]]*1000000000</f>
+        <v>1000</v>
+      </c>
+      <c r="E5" s="8">
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1*256</f>
         <v>2.5599999999999999E-4</v>
       </c>
-      <c r="E5" s="5">
+      <c r="F5" s="5">
         <f>Constants!$B$2/Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>78.125</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <f>FLOOR(Tableau1[[#This Row],[Number of TOF]], 1)</f>
         <v>78</v>
       </c>
-      <c r="G5" s="6">
+      <c r="H5" s="6">
         <f>Tableau1[[#This Row],[Integer num TOF]]*Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>1.9968E-2</v>
       </c>
-      <c r="H5" s="9">
+      <c r="I5" s="9">
         <f>(Constants!$B$2-Tableau1[[#This Row],[Achievable period (s)]])/Constants!$B$2</f>
         <v>1.6000000000000389E-3</v>
       </c>
-      <c r="I5" s="10">
+      <c r="J5" s="10">
         <f>Tableau1[[#This Row],[Tick duration (s)]]/Tableau1[[#This Row],[Achievable period (s)]]</f>
         <v>5.0080128205128203E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="12">
         <f>POWER(2,Tableau1[[#This Row],[Prescaler idx]])</f>
         <v>32</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="13">
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1</f>
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="11">
+        <f>Tableau1[[#This Row],[Tick duration (s)]]*1000000000</f>
+        <v>2000</v>
+      </c>
+      <c r="E6" s="14">
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1*256</f>
         <v>5.1199999999999998E-4</v>
       </c>
-      <c r="E6" s="5">
+      <c r="F6" s="15">
         <f>Constants!$B$2/Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>39.0625</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="16">
         <f>FLOOR(Tableau1[[#This Row],[Number of TOF]], 1)</f>
         <v>39</v>
       </c>
-      <c r="G6" s="6">
+      <c r="H6" s="17">
         <f>Tableau1[[#This Row],[Integer num TOF]]*Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>1.9968E-2</v>
       </c>
-      <c r="H6" s="9">
+      <c r="I6" s="18">
         <f>(Constants!$B$2-Tableau1[[#This Row],[Achievable period (s)]])/Constants!$B$2</f>
         <v>1.6000000000000389E-3</v>
       </c>
-      <c r="I6" s="10">
+      <c r="J6" s="19">
         <f>Tableau1[[#This Row],[Tick duration (s)]]/Tableau1[[#This Row],[Achievable period (s)]]</f>
         <v>1.0016025641025641E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -785,32 +854,36 @@
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1</f>
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="3">
+        <f>Tableau1[[#This Row],[Tick duration (s)]]*1000000000</f>
+        <v>4000</v>
+      </c>
+      <c r="E7" s="8">
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1*256</f>
         <v>1.024E-3</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <f>Constants!$B$2/Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>19.53125</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <f>FLOOR(Tableau1[[#This Row],[Number of TOF]], 1)</f>
         <v>19</v>
       </c>
-      <c r="G7" s="6">
+      <c r="H7" s="6">
         <f>Tableau1[[#This Row],[Integer num TOF]]*Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>1.9455999999999998E-2</v>
       </c>
-      <c r="H7" s="9">
+      <c r="I7" s="9">
         <f>(Constants!$B$2-Tableau1[[#This Row],[Achievable period (s)]])/Constants!$B$2</f>
         <v>2.7200000000000141E-2</v>
       </c>
-      <c r="I7" s="10">
+      <c r="J7" s="10">
         <f>Tableau1[[#This Row],[Tick duration (s)]]/Tableau1[[#This Row],[Achievable period (s)]]</f>
         <v>2.0559210526315791E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -822,32 +895,36 @@
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1</f>
         <v>7.9999999999999996E-6</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="3">
+        <f>Tableau1[[#This Row],[Tick duration (s)]]*1000000000</f>
+        <v>8000</v>
+      </c>
+      <c r="E8" s="8">
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1*256</f>
         <v>2.0479999999999999E-3</v>
       </c>
-      <c r="E8" s="5">
+      <c r="F8" s="5">
         <f>Constants!$B$2/Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>9.765625</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <f>FLOOR(Tableau1[[#This Row],[Number of TOF]], 1)</f>
         <v>9</v>
       </c>
-      <c r="G8" s="6">
+      <c r="H8" s="6">
         <f>Tableau1[[#This Row],[Integer num TOF]]*Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>1.8432E-2</v>
       </c>
-      <c r="H8" s="9">
+      <c r="I8" s="9">
         <f>(Constants!$B$2-Tableau1[[#This Row],[Achievable period (s)]])/Constants!$B$2</f>
         <v>7.8399999999999997E-2</v>
       </c>
-      <c r="I8" s="10">
+      <c r="J8" s="10">
         <f>Tableau1[[#This Row],[Tick duration (s)]]/Tableau1[[#This Row],[Achievable period (s)]]</f>
         <v>4.3402777777777775E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -859,32 +936,36 @@
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1</f>
         <v>1.5999999999999999E-5</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="3">
+        <f>Tableau1[[#This Row],[Tick duration (s)]]*1000000000</f>
+        <v>16000</v>
+      </c>
+      <c r="E9" s="8">
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1*256</f>
         <v>4.0959999999999998E-3</v>
       </c>
-      <c r="E9" s="5">
+      <c r="F9" s="5">
         <f>Constants!$B$2/Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>4.8828125</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <f>FLOOR(Tableau1[[#This Row],[Number of TOF]], 1)</f>
         <v>4</v>
       </c>
-      <c r="G9" s="6">
+      <c r="H9" s="6">
         <f>Tableau1[[#This Row],[Integer num TOF]]*Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>1.6383999999999999E-2</v>
       </c>
-      <c r="H9" s="9">
+      <c r="I9" s="9">
         <f>(Constants!$B$2-Tableau1[[#This Row],[Achievable period (s)]])/Constants!$B$2</f>
         <v>0.18080000000000004</v>
       </c>
-      <c r="I9" s="10">
+      <c r="J9" s="10">
         <f>Tableau1[[#This Row],[Tick duration (s)]]/Tableau1[[#This Row],[Achievable period (s)]]</f>
         <v>9.765625E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -896,32 +977,36 @@
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1</f>
         <v>3.1999999999999999E-5</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="3">
+        <f>Tableau1[[#This Row],[Tick duration (s)]]*1000000000</f>
+        <v>32000</v>
+      </c>
+      <c r="E10" s="8">
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1*256</f>
         <v>8.1919999999999996E-3</v>
       </c>
-      <c r="E10" s="5">
+      <c r="F10" s="5">
         <f>Constants!$B$2/Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>2.44140625</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <f>FLOOR(Tableau1[[#This Row],[Number of TOF]], 1)</f>
         <v>2</v>
       </c>
-      <c r="G10" s="6">
+      <c r="H10" s="6">
         <f>Tableau1[[#This Row],[Integer num TOF]]*Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>1.6383999999999999E-2</v>
       </c>
-      <c r="H10" s="9">
+      <c r="I10" s="9">
         <f>(Constants!$B$2-Tableau1[[#This Row],[Achievable period (s)]])/Constants!$B$2</f>
         <v>0.18080000000000004</v>
       </c>
-      <c r="I10" s="10">
+      <c r="J10" s="10">
         <f>Tableau1[[#This Row],[Tick duration (s)]]/Tableau1[[#This Row],[Achievable period (s)]]</f>
         <v>1.953125E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -933,27 +1018,31 @@
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1</f>
         <v>6.3999999999999997E-5</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="3">
+        <f>Tableau1[[#This Row],[Tick duration (s)]]*1000000000</f>
+        <v>64000</v>
+      </c>
+      <c r="E11" s="8">
         <f>Tableau1[[#This Row],[Prescaler]]/Constants!$B$1*256</f>
         <v>1.6383999999999999E-2</v>
       </c>
-      <c r="E11" s="5">
+      <c r="F11" s="5">
         <f>Constants!$B$2/Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>1.220703125</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <f>FLOOR(Tableau1[[#This Row],[Number of TOF]], 1)</f>
         <v>1</v>
       </c>
-      <c r="G11" s="6">
+      <c r="H11" s="6">
         <f>Tableau1[[#This Row],[Integer num TOF]]*Tableau1[[#This Row],[TOF Period (s)]]</f>
         <v>1.6383999999999999E-2</v>
       </c>
-      <c r="H11" s="9">
+      <c r="I11" s="9">
         <f>(Constants!$B$2-Tableau1[[#This Row],[Achievable period (s)]])/Constants!$B$2</f>
         <v>0.18080000000000004</v>
       </c>
-      <c r="I11" s="10">
+      <c r="J11" s="10">
         <f>Tableau1[[#This Row],[Tick duration (s)]]/Tableau1[[#This Row],[Achievable period (s)]]</f>
         <v>3.90625E-3</v>
       </c>
@@ -971,7 +1060,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>